<commit_message>
update for new ticker structure and input/output chart
</commit_message>
<xml_diff>
--- a/commo_list.xlsx
+++ b/commo_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duynguyen/Library/CloudStorage/GoogleDrive-nkduy96@gmail.com/My Drive/Python/Commo Dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198060AC-3053-D347-983E-B3C5EC5FEE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB44CF3-5842-1F45-BF30-287DB4B305A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37840" yWindow="620" windowWidth="28040" windowHeight="26960" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
+    <workbookView xWindow="37900" yWindow="620" windowWidth="28040" windowHeight="26960" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="commo_list" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="122">
   <si>
     <t>Sector</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>Long Steel</t>
-  </si>
-  <si>
-    <t>VN</t>
   </si>
   <si>
     <t>Long steel HPG</t>
@@ -1279,9 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6211FC7B-C9F6-474D-869C-41D822FE504E}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1373,7 +1368,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1415,7 +1410,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1429,7 +1424,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1443,7 +1438,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1485,7 +1480,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1499,7 +1494,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1555,7 +1550,7 @@
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,7 +1564,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1583,7 +1578,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1625,7 +1620,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1639,7 +1634,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1790,10 +1785,10 @@
         <v>50</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1807,7 +1802,7 @@
         <v>19</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1821,7 +1816,7 @@
         <v>19</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1829,13 +1824,13 @@
         <v>49</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1843,13 +1838,13 @@
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1857,13 +1852,13 @@
         <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1871,13 +1866,13 @@
         <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1885,13 +1880,13 @@
         <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1899,517 +1894,517 @@
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update logic for loading quick view using st.fragment
</commit_message>
<xml_diff>
--- a/commo_list.xlsx
+++ b/commo_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duynguyen/Library/CloudStorage/GoogleDrive-nkduy96@gmail.com/My Drive/Python/Commo Dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7961A1B-B028-E548-AAAB-7E82183E0F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF2A03-8926-384A-8AFA-33EF55748E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="620" windowWidth="28040" windowHeight="26960" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
   </bookViews>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6211FC7B-C9F6-474D-869C-41D822FE504E}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="178" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update new quick view
</commit_message>
<xml_diff>
--- a/commo_list.xlsx
+++ b/commo_list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duynguyen/Library/CloudStorage/GoogleDrive-nkduy96@gmail.com/My Drive/Python/Commo Dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF2A03-8926-384A-8AFA-33EF55748E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2410D1C3-947F-A346-9954-B24613E6524E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="620" windowWidth="28040" windowHeight="26960" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
+    <workbookView xWindow="28480" yWindow="620" windowWidth="28040" windowHeight="26960" activeTab="1" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="commo_list" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="182">
   <si>
     <t>Sector</t>
   </si>
@@ -384,6 +385,201 @@
   </si>
   <si>
     <t>Milk</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Is_Classified</t>
+  </si>
+  <si>
+    <t>BBG</t>
+  </si>
+  <si>
+    <t>Non_BBG</t>
+  </si>
+  <si>
+    <t>ANV_China_Value</t>
+  </si>
+  <si>
+    <t>ANV_Total_ASP</t>
+  </si>
+  <si>
+    <t>ANV_Total_Value</t>
+  </si>
+  <si>
+    <t>ANV_USA_Value</t>
+  </si>
+  <si>
+    <t>Aus Coal</t>
+  </si>
+  <si>
+    <t>Cash Cost</t>
+  </si>
+  <si>
+    <t>Cash Cost Moving Avg 15</t>
+  </si>
+  <si>
+    <t>China Bismuth</t>
+  </si>
+  <si>
+    <t>China Fluorspar</t>
+  </si>
+  <si>
+    <t>China HRC Margin</t>
+  </si>
+  <si>
+    <t>China HRC Moving Avg 15</t>
+  </si>
+  <si>
+    <t>China LS</t>
+  </si>
+  <si>
+    <t>China LS Moving Avg 15</t>
+  </si>
+  <si>
+    <t>China Thermal Coal</t>
+  </si>
+  <si>
+    <t>China Urea</t>
+  </si>
+  <si>
+    <t>China Urea Futures</t>
+  </si>
+  <si>
+    <t>China Urea Prill</t>
+  </si>
+  <si>
+    <t>Container Volume Central</t>
+  </si>
+  <si>
+    <t>Container Volume North</t>
+  </si>
+  <si>
+    <t>Container Volume South</t>
+  </si>
+  <si>
+    <t>Container Volume Total</t>
+  </si>
+  <si>
+    <t>EAF</t>
+  </si>
+  <si>
+    <t>EAF Moving Avg 15</t>
+  </si>
+  <si>
+    <t>Global Urea Spread</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>HRC China</t>
+  </si>
+  <si>
+    <t>IDI_Total_ASP</t>
+  </si>
+  <si>
+    <t>IDI_Total_Value</t>
+  </si>
+  <si>
+    <t>IDI_USA_ASP</t>
+  </si>
+  <si>
+    <t>IDI_USA_Value</t>
+  </si>
+  <si>
+    <t>Indo Urea</t>
+  </si>
+  <si>
+    <t>International Rig Count</t>
+  </si>
+  <si>
+    <t>Long steel China</t>
+  </si>
+  <si>
+    <t>MOP China</t>
+  </si>
+  <si>
+    <t>Malting Barley - Australia</t>
+  </si>
+  <si>
+    <t>Marine Fuel Oil</t>
+  </si>
+  <si>
+    <t>PVC Contract SEA</t>
+  </si>
+  <si>
+    <t>Palm Oil</t>
+  </si>
+  <si>
+    <t>Potash US</t>
+  </si>
+  <si>
+    <t>SE Asia PS</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Spot China HRC</t>
+  </si>
+  <si>
+    <t>Spot China LS</t>
+  </si>
+  <si>
+    <t>Spot VN HRC</t>
+  </si>
+  <si>
+    <t>Spot VN LS</t>
+  </si>
+  <si>
+    <t>US Amonia</t>
+  </si>
+  <si>
+    <t>US Crack Spread</t>
+  </si>
+  <si>
+    <t>US Rig Count</t>
+  </si>
+  <si>
+    <t>Urea Middle East</t>
+  </si>
+  <si>
+    <t>Urea Simulated Spread</t>
+  </si>
+  <si>
+    <t>Urea US</t>
+  </si>
+  <si>
+    <t>VHC_China_ASP</t>
+  </si>
+  <si>
+    <t>VHC_China_Value</t>
+  </si>
+  <si>
+    <t>VHC_Total_Value</t>
+  </si>
+  <si>
+    <t>VHC_USA_Value</t>
+  </si>
+  <si>
+    <t>VN HRC</t>
+  </si>
+  <si>
+    <t>VN HRC Moving Avg 15</t>
+  </si>
+  <si>
+    <t>VN LS</t>
+  </si>
+  <si>
+    <t>VN LS Moving Avg 15</t>
+  </si>
+  <si>
+    <t>Very Low Sulfur Fuel Oil</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6211FC7B-C9F6-474D-869C-41D822FE504E}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="178" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="178" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2342,4 +2538,1504 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B43E1FD-A1E9-044B-8C54-F187F44FDBA8}">
+  <dimension ref="A1:C135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>143</v>
+      </c>
+      <c r="B53" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>88</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" t="s">
+        <v>121</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>51</v>
+      </c>
+      <c r="B79" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" t="s">
+        <v>120</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" t="s">
+        <v>120</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" t="s">
+        <v>120</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" t="s">
+        <v>121</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" t="s">
+        <v>121</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>99</v>
+      </c>
+      <c r="B86" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>64</v>
+      </c>
+      <c r="B87" t="s">
+        <v>121</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" t="s">
+        <v>120</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" t="s">
+        <v>120</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>159</v>
+      </c>
+      <c r="B91" t="s">
+        <v>120</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92" t="s">
+        <v>121</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" t="s">
+        <v>120</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" t="s">
+        <v>120</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>43</v>
+      </c>
+      <c r="B95" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>161</v>
+      </c>
+      <c r="B96" t="s">
+        <v>120</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>68</v>
+      </c>
+      <c r="B97" t="s">
+        <v>120</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" t="s">
+        <v>120</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>162</v>
+      </c>
+      <c r="B99" t="s">
+        <v>120</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" t="s">
+        <v>120</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" t="s">
+        <v>121</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>82</v>
+      </c>
+      <c r="B102" t="s">
+        <v>121</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>163</v>
+      </c>
+      <c r="B103" t="s">
+        <v>121</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>164</v>
+      </c>
+      <c r="B104" t="s">
+        <v>121</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>165</v>
+      </c>
+      <c r="B105" t="s">
+        <v>121</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>166</v>
+      </c>
+      <c r="B106" t="s">
+        <v>121</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" t="s">
+        <v>120</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>39</v>
+      </c>
+      <c r="B108" t="s">
+        <v>121</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>167</v>
+      </c>
+      <c r="B109" t="s">
+        <v>120</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>168</v>
+      </c>
+      <c r="B110" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>60</v>
+      </c>
+      <c r="B111" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>103</v>
+      </c>
+      <c r="B112" t="s">
+        <v>120</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>169</v>
+      </c>
+      <c r="B113" t="s">
+        <v>120</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>25</v>
+      </c>
+      <c r="B114" t="s">
+        <v>120</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" t="s">
+        <v>120</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>27</v>
+      </c>
+      <c r="B116" t="s">
+        <v>120</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>170</v>
+      </c>
+      <c r="B117" t="s">
+        <v>120</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>171</v>
+      </c>
+      <c r="B118" t="s">
+        <v>121</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>172</v>
+      </c>
+      <c r="B119" t="s">
+        <v>120</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>173</v>
+      </c>
+      <c r="B120" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>174</v>
+      </c>
+      <c r="B121" t="s">
+        <v>121</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>115</v>
+      </c>
+      <c r="B122" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>175</v>
+      </c>
+      <c r="B123" t="s">
+        <v>121</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>100</v>
+      </c>
+      <c r="B124" t="s">
+        <v>121</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>176</v>
+      </c>
+      <c r="B125" t="s">
+        <v>121</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>177</v>
+      </c>
+      <c r="B126" t="s">
+        <v>121</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>178</v>
+      </c>
+      <c r="B127" t="s">
+        <v>121</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>179</v>
+      </c>
+      <c r="B128" t="s">
+        <v>121</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>180</v>
+      </c>
+      <c r="B129" t="s">
+        <v>121</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>181</v>
+      </c>
+      <c r="B130" t="s">
+        <v>120</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" t="s">
+        <v>120</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>84</v>
+      </c>
+      <c r="B132" t="s">
+        <v>121</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>36</v>
+      </c>
+      <c r="B133" t="s">
+        <v>121</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>108</v>
+      </c>
+      <c r="B134" t="s">
+        <v>120</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>109</v>
+      </c>
+      <c r="B135" t="s">
+        <v>120</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new commo list and bug fix. getting ready for full live data
</commit_message>
<xml_diff>
--- a/commo_list.xlsx
+++ b/commo_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duynguyen/Library/CloudStorage/GoogleDrive-nkduy96@gmail.com/My Drive/Python/Commo Dash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Python\Commo Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2410D1C3-947F-A346-9954-B24613E6524E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7B15C6-8FC4-4E41-8903-72803CEA65BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28480" yWindow="620" windowWidth="28040" windowHeight="26960" activeTab="1" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
+    <workbookView xWindow="10170" yWindow="2655" windowWidth="17910" windowHeight="14325" xr2:uid="{DFB136D8-C29C-AF48-B48A-F9D91324BA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="commo_list" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="184">
   <si>
     <t>Sector</t>
   </si>
@@ -147,18 +147,12 @@
     <t>Yellow phosphorus - China</t>
   </si>
   <si>
-    <t>P4 Rock</t>
-  </si>
-  <si>
     <t>Phosphate rock</t>
   </si>
   <si>
     <t>Thermal phosphoric acid - China</t>
   </si>
   <si>
-    <t>Yellow phosphorus - DGC</t>
-  </si>
-  <si>
     <t>PVC</t>
   </si>
   <si>
@@ -580,6 +574,18 @@
   </si>
   <si>
     <t>Very Low Sulfur Fuel Oil</t>
+  </si>
+  <si>
+    <t>Ure_DCM</t>
+  </si>
+  <si>
+    <t>Ure_DPM</t>
+  </si>
+  <si>
+    <t>Yellow phosphorus China</t>
+  </si>
+  <si>
+    <t>Thermal phosphoric acid China</t>
   </si>
 </sst>
 </file>
@@ -1455,22 +1461,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6211FC7B-C9F6-474D-869C-41D822FE504E}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="178" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.875" style="1"/>
     <col min="4" max="4" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1498,7 +1504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1551,38 +1557,38 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1590,55 +1596,55 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1646,13 +1652,13 @@
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1660,13 +1666,13 @@
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1674,13 +1680,13 @@
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1691,38 +1697,38 @@
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1733,38 +1739,38 @@
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1772,13 +1778,13 @@
         <v>29</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1786,752 +1792,654 @@
         <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="B49" s="1" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D74" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2544,1492 +2452,1492 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B43E1FD-A1E9-044B-8C54-F187F44FDBA8}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>120</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>121</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>122</v>
       </c>
-      <c r="B5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>123</v>
       </c>
-      <c r="B6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>124</v>
       </c>
-      <c r="B7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>126</v>
-      </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>127</v>
       </c>
-      <c r="B23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>129</v>
-      </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>130</v>
       </c>
-      <c r="B28" t="s">
-        <v>120</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>131</v>
       </c>
-      <c r="B30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>132</v>
       </c>
-      <c r="B31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>133</v>
       </c>
-      <c r="B32" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>134</v>
       </c>
-      <c r="B33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" t="s">
-        <v>120</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>136</v>
-      </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>137</v>
       </c>
-      <c r="B39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>138</v>
       </c>
-      <c r="B40" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>139</v>
       </c>
-      <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>140</v>
       </c>
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>141</v>
-      </c>
-      <c r="B43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>142</v>
-      </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>145</v>
       </c>
-      <c r="B57" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>146</v>
       </c>
-      <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>147</v>
       </c>
-      <c r="B59" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" t="s">
-        <v>121</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>55</v>
-      </c>
-      <c r="B62" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>88</v>
-      </c>
-      <c r="B64" t="s">
-        <v>121</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>90</v>
-      </c>
-      <c r="B65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" t="s">
-        <v>121</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" t="s">
-        <v>121</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" t="s">
-        <v>121</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" t="s">
-        <v>121</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>148</v>
       </c>
-      <c r="B71" t="s">
-        <v>121</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B73" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>149</v>
       </c>
-      <c r="B72" t="s">
-        <v>121</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>150</v>
       </c>
-      <c r="B73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>151</v>
       </c>
-      <c r="B74" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>152</v>
-      </c>
-      <c r="B75" t="s">
-        <v>120</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>153</v>
-      </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>49</v>
+      </c>
+      <c r="B79" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>153</v>
+      </c>
+      <c r="B80" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>154</v>
       </c>
-      <c r="B78" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>51</v>
-      </c>
-      <c r="B79" t="s">
-        <v>121</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="B81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>155</v>
       </c>
-      <c r="B80" t="s">
-        <v>120</v>
-      </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="B83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>62</v>
+      </c>
+      <c r="B87" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B88" t="s">
+        <v>118</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>156</v>
       </c>
-      <c r="B81" t="s">
-        <v>120</v>
-      </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>79</v>
-      </c>
-      <c r="B82" t="s">
-        <v>120</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="B89" t="s">
+        <v>118</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>157</v>
       </c>
-      <c r="B83" t="s">
-        <v>120</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>97</v>
-      </c>
-      <c r="B84" t="s">
-        <v>121</v>
-      </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>98</v>
-      </c>
-      <c r="B85" t="s">
-        <v>121</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>99</v>
-      </c>
-      <c r="B86" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>64</v>
-      </c>
-      <c r="B87" t="s">
-        <v>121</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>63</v>
-      </c>
-      <c r="B88" t="s">
-        <v>120</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>37</v>
+      </c>
+      <c r="B92" t="s">
+        <v>119</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>158</v>
       </c>
-      <c r="B89" t="s">
-        <v>120</v>
-      </c>
-      <c r="C89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>42</v>
-      </c>
-      <c r="B90" t="s">
-        <v>120</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="B93" t="s">
+        <v>118</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>41</v>
+      </c>
+      <c r="B95" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>159</v>
       </c>
-      <c r="B91" t="s">
-        <v>120</v>
-      </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>38</v>
-      </c>
-      <c r="B92" t="s">
-        <v>121</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="B96" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" t="s">
+        <v>118</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>160</v>
       </c>
-      <c r="B93" t="s">
-        <v>120</v>
-      </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>85</v>
-      </c>
-      <c r="B94" t="s">
-        <v>120</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>43</v>
-      </c>
-      <c r="B95" t="s">
-        <v>120</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>161</v>
-      </c>
-      <c r="B96" t="s">
-        <v>120</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>68</v>
-      </c>
-      <c r="B97" t="s">
-        <v>120</v>
-      </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>74</v>
-      </c>
-      <c r="B98" t="s">
-        <v>120</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>162</v>
-      </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B101" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B102" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>161</v>
+      </c>
+      <c r="B103" t="s">
+        <v>119</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>162</v>
+      </c>
+      <c r="B104" t="s">
+        <v>119</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>163</v>
       </c>
-      <c r="B103" t="s">
-        <v>121</v>
-      </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="B105" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>164</v>
       </c>
-      <c r="B104" t="s">
-        <v>121</v>
-      </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="B106" t="s">
+        <v>119</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>84</v>
+      </c>
+      <c r="B107" t="s">
+        <v>118</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>38</v>
+      </c>
+      <c r="B108" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>165</v>
       </c>
-      <c r="B105" t="s">
-        <v>121</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="B109" t="s">
+        <v>118</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>166</v>
       </c>
-      <c r="B106" t="s">
-        <v>121</v>
-      </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>86</v>
-      </c>
-      <c r="B107" t="s">
-        <v>120</v>
-      </c>
-      <c r="C107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>39</v>
-      </c>
-      <c r="B108" t="s">
-        <v>121</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="B110" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>58</v>
+      </c>
+      <c r="B111" t="s">
+        <v>119</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>101</v>
+      </c>
+      <c r="B112" t="s">
+        <v>118</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>167</v>
       </c>
-      <c r="B109" t="s">
-        <v>120</v>
-      </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>168</v>
-      </c>
-      <c r="B110" t="s">
-        <v>120</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>60</v>
-      </c>
-      <c r="B111" t="s">
-        <v>121</v>
-      </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>103</v>
-      </c>
-      <c r="B112" t="s">
-        <v>120</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>169</v>
-      </c>
       <c r="B113" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C113">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>25</v>
       </c>
       <c r="B114" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>26</v>
       </c>
       <c r="B115" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>27</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>168</v>
+      </c>
+      <c r="B117" t="s">
+        <v>118</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>169</v>
+      </c>
+      <c r="B118" t="s">
+        <v>119</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>170</v>
       </c>
-      <c r="B117" t="s">
-        <v>120</v>
-      </c>
-      <c r="C117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="B119" t="s">
+        <v>118</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>171</v>
       </c>
-      <c r="B118" t="s">
-        <v>121</v>
-      </c>
-      <c r="C118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="B120" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>172</v>
       </c>
-      <c r="B119" t="s">
-        <v>120</v>
-      </c>
-      <c r="C119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="B121" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>113</v>
+      </c>
+      <c r="B122" t="s">
+        <v>119</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>173</v>
       </c>
-      <c r="B120" t="s">
-        <v>121</v>
-      </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="B123" t="s">
+        <v>119</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>98</v>
+      </c>
+      <c r="B124" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>174</v>
       </c>
-      <c r="B121" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>115</v>
-      </c>
-      <c r="B122" t="s">
-        <v>121</v>
-      </c>
-      <c r="C122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="B125" t="s">
+        <v>119</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>175</v>
       </c>
-      <c r="B123" t="s">
-        <v>121</v>
-      </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>100</v>
-      </c>
-      <c r="B124" t="s">
-        <v>121</v>
-      </c>
-      <c r="C124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="B126" t="s">
+        <v>119</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>176</v>
       </c>
-      <c r="B125" t="s">
-        <v>121</v>
-      </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="B127" t="s">
+        <v>119</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>177</v>
       </c>
-      <c r="B126" t="s">
-        <v>121</v>
-      </c>
-      <c r="C126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="B128" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>178</v>
       </c>
-      <c r="B127" t="s">
-        <v>121</v>
-      </c>
-      <c r="C127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="B129" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>179</v>
       </c>
-      <c r="B128" t="s">
-        <v>121</v>
-      </c>
-      <c r="C128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>180</v>
-      </c>
-      <c r="B129" t="s">
-        <v>121</v>
-      </c>
-      <c r="C129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>181</v>
-      </c>
       <c r="B130" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C130">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>7</v>
       </c>
       <c r="B131" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B132" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>36</v>
       </c>
       <c r="B133" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C135">
         <v>1</v>

</xml_diff>